<commit_message>
fixes -1 min in corrected metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_daily_corrected_passage.xlsx
+++ b/data-raw/metadata/yuba_daily_corrected_passage.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/SRJPE/EDI/jpe-yuba-adult-edi/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-yuba-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B143CC8-31F2-6949-8144-50D459249406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAF3B33-4587-C143-BBD8-7F266DFF0178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29400" yWindow="660" windowWidth="31620" windowHeight="22720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
     <sheet name="code_definitions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterate="1"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mjgCtONQL+sZFXm0/U8uf/vdSvo/w=="/>
@@ -464,9 +464,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -657,7 +657,7 @@
       <c r="J4" s="14"/>
       <c r="K4" s="13"/>
       <c r="L4" s="14">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="14">
         <v>538</v>

</xml_diff>